<commit_message>
02/03/2023 * Update of the documentation
</commit_message>
<xml_diff>
--- a/doc/endpoint_address.xlsx
+++ b/doc/endpoint_address.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATHENA_X-IFU\Documents\Noemie2020\Documents_projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurent/work/work_vhdl/RAS/ras-a75-fw/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0461C7AE-9A87-984B-BBB3-94CDA85F31A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="42100" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="98">
   <si>
     <t>nom</t>
   </si>
@@ -318,15 +319,12 @@
   </si>
   <si>
     <t>register(0)</t>
-  </si>
-  <si>
-    <t>Version Firmware : ras-a75-fw 1.3.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,18 +350,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -382,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,32 +654,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D24" sqref="D24"/>
+      <selection pane="topRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" customWidth="1"/>
+    <col min="24" max="24" width="15.5" customWidth="1"/>
+    <col min="25" max="25" width="15.83203125" customWidth="1"/>
+    <col min="26" max="26" width="15.1640625" customWidth="1"/>
     <col min="27" max="27" width="15" customWidth="1"/>
-    <col min="28" max="28" width="14.7109375" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" customWidth="1"/>
     <col min="29" max="29" width="15" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" customWidth="1"/>
-    <col min="34" max="34" width="14.28515625" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" customWidth="1"/>
+    <col min="31" max="31" width="14.6640625" customWidth="1"/>
+    <col min="32" max="33" width="14.5" customWidth="1"/>
+    <col min="34" max="34" width="14.33203125" customWidth="1"/>
+    <col min="35" max="35" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -790,7 +781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -897,7 +888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -1004,7 +995,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -1108,7 +1099,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -1215,7 +1206,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
@@ -1322,10 +1313,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>98</v>
-      </c>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>

</xml_diff>

<commit_message>
16/01/2024 (Updated to comply with new Kazu's row electronics) * Uses Opal Kelly 200MHz clock * Makes, uses and sends a 122.88MHz master clock
</commit_message>
<xml_diff>
--- a/doc/endpoint_address.xlsx
+++ b/doc/endpoint_address.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATHENA_X-IFU\Documents\Noemie2020\Documents_projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurent/work/work_vhdl/RAS/ras-a75-fw/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0461C7AE-9A87-984B-BBB3-94CDA85F31A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="42100" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="98">
   <si>
     <t>nom</t>
   </si>
@@ -318,15 +319,12 @@
   </si>
   <si>
     <t>register(0)</t>
-  </si>
-  <si>
-    <t>Version Firmware : ras-a75-fw 1.3.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,18 +350,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -382,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,32 +654,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D24" sqref="D24"/>
+      <selection pane="topRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" customWidth="1"/>
+    <col min="24" max="24" width="15.5" customWidth="1"/>
+    <col min="25" max="25" width="15.83203125" customWidth="1"/>
+    <col min="26" max="26" width="15.1640625" customWidth="1"/>
     <col min="27" max="27" width="15" customWidth="1"/>
-    <col min="28" max="28" width="14.7109375" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" customWidth="1"/>
     <col min="29" max="29" width="15" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" customWidth="1"/>
-    <col min="34" max="34" width="14.28515625" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" customWidth="1"/>
+    <col min="31" max="31" width="14.6640625" customWidth="1"/>
+    <col min="32" max="33" width="14.5" customWidth="1"/>
+    <col min="34" max="34" width="14.33203125" customWidth="1"/>
+    <col min="35" max="35" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -790,7 +781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -897,7 +888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -1004,7 +995,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -1108,7 +1099,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -1215,7 +1206,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
@@ -1322,10 +1313,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>98</v>
-      </c>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>

</xml_diff>